<commit_message>
1.加入dijikey product description，product status
</commit_message>
<xml_diff>
--- a/TSumNvmNdt/IC_stock.xlsx
+++ b/TSumNvmNdt/IC_stock.xlsx
@@ -32,6 +32,55 @@
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg1TkxUMUc=" sheetId="24" state="visible" r:id="rId24"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg1TkxUM0c=" sheetId="25" state="visible" r:id="rId25"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg1TkxXRlQxRw==" sheetId="26" state="visible" r:id="rId26"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg1TkxXRlQzRw==" sheetId="27" state="visible" r:id="rId27"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg5TkxUMUc=" sheetId="28" state="visible" r:id="rId28"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg5TkxUM0c=" sheetId="29" state="visible" r:id="rId29"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg5TkxXRlQxRw==" sheetId="30" state="visible" r:id="rId30"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1NDg5TkxXRlQzRw==" sheetId="31" state="visible" r:id="rId31"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUyTkxUMUc=" sheetId="32" state="visible" r:id="rId32"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUyTkxXRlQxRw==" sheetId="33" state="visible" r:id="rId33"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUzTkxUMUc=" sheetId="34" state="visible" r:id="rId34"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUzTkxXRlQxRw==" sheetId="35" state="visible" r:id="rId35"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUzTlQxRw==" sheetId="36" state="visible" r:id="rId36"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODUzTldGVDFH" sheetId="37" state="visible" r:id="rId37"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODczTkxUMUc=" sheetId="38" state="visible" r:id="rId38"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODczTkxXRlQxRw==" sheetId="39" state="visible" r:id="rId39"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc1TkxUMUc=" sheetId="40" state="visible" r:id="rId40"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc1TkxUM0c=" sheetId="41" state="visible" r:id="rId41"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc1TkxXRlQxRw==" sheetId="42" state="visible" r:id="rId42"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc1TkxXRlQzRw==" sheetId="43" state="visible" r:id="rId43"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc3TkxUMUc=" sheetId="44" state="visible" r:id="rId44"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc3TkxUM0c=" sheetId="45" state="visible" r:id="rId45"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc3TkxXRlQxRw==" sheetId="46" state="visible" r:id="rId46"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1ODc3TkxXRlQzRw==" sheetId="47" state="visible" r:id="rId47"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRkQ1QzQ3ME5MV0ZUMUc=" sheetId="48" state="visible" r:id="rId48"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0ODQxTlQxRw==" sheetId="49" state="visible" r:id="rId49"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0ODQxTldGVDFH" sheetId="50" state="visible" r:id="rId50"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzAxTlQzRw==" sheetId="51" state="visible" r:id="rId51"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzAxTldGVDNH" sheetId="52" state="visible" r:id="rId52"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzAzTlQzRw==" sheetId="53" state="visible" r:id="rId53"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzAzTldGVDNH" sheetId="54" state="visible" r:id="rId54"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzA1TlQzRw==" sheetId="55" state="visible" r:id="rId55"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzA1TldGVDNH" sheetId="56" state="visible" r:id="rId56"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzMxME5UM0c=" sheetId="57" state="visible" r:id="rId57"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM0QzMxME5XRlQzRw==" sheetId="58" state="visible" r:id="rId58"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODI2TkxUMUc=" sheetId="59" state="visible" r:id="rId59"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODI2TkxUM0c=" sheetId="60" state="visible" r:id="rId60"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODI2TkxXRlQxRw==" sheetId="61" state="visible" r:id="rId61"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODI2TkxXRlQzRw==" sheetId="62" state="visible" r:id="rId62"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMwTkxUMUc=" sheetId="63" state="visible" r:id="rId63"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMwTkxUM0c=" sheetId="64" state="visible" r:id="rId64"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMwTkxXRlQzRw==" sheetId="65" state="visible" r:id="rId65"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMyTkxUMUc=" sheetId="66" state="visible" r:id="rId66"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMyTkxUM0c=" sheetId="67" state="visible" r:id="rId67"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMzTlQxRw==" sheetId="68" state="visible" r:id="rId68"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODMzTldGVDFH" sheetId="69" state="visible" r:id="rId69"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODM0TkxUMUc=" sheetId="70" state="visible" r:id="rId70"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODM0TkxUM0c=" sheetId="71" state="visible" r:id="rId71"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODM0TkxXRlQzRw==" sheetId="72" state="visible" r:id="rId72"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODQ0TkxUMUc=" sheetId="73" state="visible" r:id="rId73"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODQ0TkxUM0c=" sheetId="74" state="visible" r:id="rId74"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="TlZNRlM1ODQ0TkxXRlQzRw==" sheetId="75" state="visible" r:id="rId75"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="0" fullCalcOnLoad="1"/>
@@ -1589,7 +1638,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetPr>
     <outlinePr summaryBelow="1" summaryRight="1"/>
@@ -1607,103 +1656,13 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A1" sqref="A1"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
-  <sheetData/>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-    <pageSetUpPr/>
-  </sheetPr>
-  <dimension ref="A1:I4"/>
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1714,7 +1673,7 @@
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>深圳市灿佳利电子科技有限公司</t>
+          <t>深圳市天地昆电子有限公司</t>
         </is>
       </c>
       <c r="B1" t="inlineStr">
@@ -1729,7 +1688,7 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>NDT451N</t>
+          <t>NVMFD5489NLT1G</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
@@ -1744,12 +1703,162 @@
       </c>
       <c r="G1" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>ON</t>
         </is>
       </c>
       <c r="H1" t="inlineStr">
         <is>
-          <t>2500</t>
+          <t>100</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>君盛豪（深圳）互联网半导体科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5489NLT3G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市安美迪升科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5489NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>1450</t>
         </is>
       </c>
       <c r="I1" t="inlineStr">
@@ -1761,7 +1870,7 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>深圳市亿芯正发电子有限公司</t>
+          <t>深圳市锦泰世纪电子有限公司</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
@@ -1776,7 +1885,7 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>NDT451N</t>
+          <t>NVMFD5489NLWFT1G</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
@@ -1791,12 +1900,143 @@
       </c>
       <c r="G2" t="inlineStr">
         <is>
-          <t>NS</t>
+          <t>ON</t>
         </is>
       </c>
       <c r="H2" t="inlineStr">
         <is>
-          <t>2800</t>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>上海旺韵电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5852NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>190</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市天地昆电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5852NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>4500</t>
         </is>
       </c>
       <c r="I2" t="inlineStr">
@@ -1808,7 +2048,7 @@
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>深圳鸿发励达科技有限公司</t>
+          <t>深圳市东翔创展电子有限公司</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
@@ -1823,7 +2063,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>NDT451N</t>
+          <t>NVMFD5852NLT1G</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -1838,12 +2078,12 @@
       </c>
       <c r="G3" t="inlineStr">
         <is>
-          <t>FSC</t>
+          <t>ON</t>
         </is>
       </c>
       <c r="H3" t="inlineStr">
         <is>
-          <t>4500</t>
+          <t>40</t>
         </is>
       </c>
       <c r="I3" t="inlineStr">
@@ -1855,6 +2095,3633 @@
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
+          <t>深圳市壮越微电子有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFD5852NLT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>684</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市国联智讯科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市亿海鸿博电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>980</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市宇星盛科技有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>原装TI</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1674</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市宏英微科技有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>3475</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>深圳市正源鸿业电子科技有限公司（原北京正源伟业电子）</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>173</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>深圳市芯通晟电子有限公司</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>深圳市驰格科技有限公司</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLT1G</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市华维微电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5853NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>643</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市天地昆电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5875NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市长润泽科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>12000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市忠发滨洋科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>192</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市众信伟业电子有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>65</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>上海旺韵电子有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>80</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市广鑫世纪电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT3G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>1051</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市中宇微科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLT3G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>642</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市创芯联盈电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>1482</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>上海旺韵电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5877NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳卓赛科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFD5C470NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>伯仲电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFD5C470NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市创海发电子有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFD5C470NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市湖盛电子有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFD5C470NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>深圳万旺达实业有限公司</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NVMFD5C470NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>原装ON</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>231</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市顺芯供应链管理有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS4841NT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>8857</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市顺芯供应链管理有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS4841NWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>2980</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet58.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet59.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet60.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet61.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市智子云科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市新数为电子科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>notSSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>6500</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市尚品诚源电子有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市金葳光电子有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>78000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>深圳市佟升电子科技有限公司</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT1G</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>18000</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet62.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市英飞翔微电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5826NLWFT3G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet63.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市鼎德丰科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5830NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>6886</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>南京金芯盛科技有限公司深圳分公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5830NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>南京金芯盛科技有限公司深圳分公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFS5830NLT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet64.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet65.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet66.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市继佳贸易有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5832NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ONSEMI</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>3000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市伊特尔电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5832NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>1969</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市金百纳电子有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFS5832NLT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>1477</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市佰一科技有限公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFS5832NLT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ON-原装现货</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>6000</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>深圳市嘉美进科技有限公司</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NVMFS5832NLT1G</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>1500</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet67.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet68.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市顺芯供应链管理有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5833NT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>54845</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet69.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市顺芯供应链管理有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5833NWFT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet70.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I10"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市欣耀兴科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市巨隆辉科技有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>SpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>7500</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳市杰盛恒芯电子有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>970</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>深圳市慧芯阳科技有限责任公司</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C4" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E4" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F4" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G4" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H4" t="inlineStr">
+        <is>
+          <t>912</t>
+        </is>
+      </c>
+      <c r="I4" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>深圳市巨隆辉科技有限公司</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C5" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D5" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E5" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F5" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G5" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H5" t="inlineStr">
+        <is>
+          <t>10500</t>
+        </is>
+      </c>
+      <c r="I5" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>深圳市胜新创科技有限公司</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D6" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E6" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F6" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G6" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H6" t="inlineStr">
+        <is>
+          <t>2545</t>
+        </is>
+      </c>
+      <c r="I6" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>深圳市亿芯正发电子有限公司</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C7" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D7" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E7" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F7" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G7" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H7" t="inlineStr">
+        <is>
+          <t>52000</t>
+        </is>
+      </c>
+      <c r="I7" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>深圳市恒意达科技有限公司</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C8" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D8" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E8" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F8" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G8" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H8" t="inlineStr">
+        <is>
+          <t>24</t>
+        </is>
+      </c>
+      <c r="I8" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>深圳市华凯诚科技有限公司</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G9" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H9" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="I9" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>深圳市两只虾电子有限公司</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>NVMFS5834NLT1G</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G10" t="inlineStr">
+        <is>
+          <t>ON/安森美原装正品</t>
+        </is>
+      </c>
+      <c r="H10" t="inlineStr">
+        <is>
+          <t>970</t>
+        </is>
+      </c>
+      <c r="I10" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet71.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet72.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet73.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市卡贝特电子有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5844NLT1G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市和信跃达电子有限公司（原北京和信拓展）</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5844NLT1G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2186</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet74.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳骏承置裕贸易有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NVMFS5844NLT3G</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>ON/安森美</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>40000</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市顺芯供应链管理有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NVMFS5844NLT3G</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>ON</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>5000</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet75.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:I4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="inlineStr">
+        <is>
+          <t>深圳市灿佳利电子科技有限公司</t>
+        </is>
+      </c>
+      <c r="B1" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C1" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>NDT451N</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F1" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G1" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="H1" t="inlineStr">
+        <is>
+          <t>2500</t>
+        </is>
+      </c>
+      <c r="I1" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>深圳市亿芯正发电子有限公司</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C2" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>NDT451N</t>
+        </is>
+      </c>
+      <c r="E2" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F2" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G2" t="inlineStr">
+        <is>
+          <t>NS</t>
+        </is>
+      </c>
+      <c r="H2" t="inlineStr">
+        <is>
+          <t>2800</t>
+        </is>
+      </c>
+      <c r="I2" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>深圳鸿发励达科技有限公司</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>notICCP</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>SSCP</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>NDT451N</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>notSpotRanking</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>notHotSell</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>FSC</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>4500</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>2023-02-22</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>深圳市金讯电科技有限公司</t>
         </is>
       </c>

</xml_diff>